<commit_message>
add insects and snails to treemap
</commit_message>
<xml_diff>
--- a/raw_data/Chart4/Daten_ZeitlicheEntwicklungen1900-2022.xlsx
+++ b/raw_data/Chart4/Daten_ZeitlicheEntwicklungen1900-2022.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karin.guedel@fhnw.ch/WebstormProjects/guedelkohler/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karin.guedel@fhnw.ch/WebstormProjects/guedelkohler/raw_data/Chart4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD56CDB-6BE3-864C-837F-C3E3372E0C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F920A5-9989-004B-9F50-E9D8C40EE141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="14540" windowHeight="16840" xr2:uid="{3090A4FA-6CEE-FC47-988A-09070F5BEFA5}"/>
+    <workbookView xWindow="420" yWindow="2780" windowWidth="28800" windowHeight="16840" xr2:uid="{3090A4FA-6CEE-FC47-988A-09070F5BEFA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>Volumen der Gesamtproduktion der Landwirtschaft</t>
   </si>
@@ -87,7 +87,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -101,6 +101,13 @@
       <color rgb="FF211D1E"/>
       <name val="Times"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -123,9 +130,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -440,18 +448,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76C37C10-B61C-5A44-BD7A-5E939DA59B8B}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="8" width="20.6640625" customWidth="1"/>
+    <col min="2" max="10" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -459,31 +467,37 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
         <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" t="s">
-        <v>11</v>
       </c>
       <c r="G1" t="s">
         <v>10</v>
       </c>
       <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1900</v>
       </c>
@@ -491,13 +505,15 @@
         <v>100</v>
       </c>
       <c r="C2">
-        <v>100</v>
+        <f>B2-100</f>
+        <v>0</v>
       </c>
       <c r="D2">
         <v>100</v>
       </c>
       <c r="E2">
-        <v>100</v>
+        <f>D2-100</f>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>100</v>
@@ -505,11 +521,17 @@
       <c r="G2">
         <v>100</v>
       </c>
-      <c r="J2">
+      <c r="H2">
+        <v>100</v>
+      </c>
+      <c r="I2">
+        <v>100</v>
+      </c>
+      <c r="L2">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1915</v>
       </c>
@@ -517,13 +539,30 @@
         <v>125</v>
       </c>
       <c r="C3">
+        <f t="shared" ref="C3:C11" si="0">B3-100</f>
+        <v>25</v>
+      </c>
+      <c r="D3">
         <v>120</v>
       </c>
-      <c r="D3">
+      <c r="E3">
+        <f t="shared" ref="E3:E11" si="1">D3-100</f>
+        <v>20</v>
+      </c>
+      <c r="F3">
         <v>96</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G3" s="2">
+        <v>96</v>
+      </c>
+      <c r="H3" s="2">
+        <v>93</v>
+      </c>
+      <c r="I3" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1930</v>
       </c>
@@ -531,16 +570,33 @@
         <v>150</v>
       </c>
       <c r="C4">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="D4">
         <v>125</v>
       </c>
-      <c r="D4">
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="F4">
         <v>94</v>
       </c>
-      <c r="J4">
+      <c r="G4" s="2">
+        <v>90</v>
+      </c>
+      <c r="H4" s="2">
+        <v>80</v>
+      </c>
+      <c r="I4" s="2">
+        <v>75</v>
+      </c>
+      <c r="L4">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1945</v>
       </c>
@@ -548,16 +604,33 @@
         <v>160</v>
       </c>
       <c r="C5">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="D5">
         <v>130</v>
       </c>
-      <c r="D5">
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="F5">
         <v>96</v>
       </c>
-      <c r="I5">
+      <c r="G5" s="2">
+        <v>85</v>
+      </c>
+      <c r="H5" s="2">
+        <v>65</v>
+      </c>
+      <c r="I5" s="2">
+        <v>60</v>
+      </c>
+      <c r="K5">
         <v>400</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1960</v>
       </c>
@@ -565,19 +638,36 @@
         <v>170</v>
       </c>
       <c r="C6">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="D6">
         <v>150</v>
       </c>
-      <c r="D6">
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="F6">
         <v>92</v>
       </c>
-      <c r="I6">
+      <c r="G6" s="2">
+        <v>80</v>
+      </c>
+      <c r="H6" s="2">
+        <v>45</v>
+      </c>
+      <c r="I6" s="2">
+        <v>40</v>
+      </c>
+      <c r="K6">
         <v>1200</v>
       </c>
-      <c r="J6">
+      <c r="L6">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1975</v>
       </c>
@@ -585,19 +675,36 @@
         <v>190</v>
       </c>
       <c r="C7">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="D7">
         <v>180</v>
       </c>
-      <c r="D7">
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="F7">
         <v>87</v>
       </c>
-      <c r="I7">
+      <c r="G7" s="2">
+        <v>70</v>
+      </c>
+      <c r="H7" s="2">
+        <v>30</v>
+      </c>
+      <c r="I7" s="2">
+        <v>20</v>
+      </c>
+      <c r="K7">
         <v>3500</v>
       </c>
-      <c r="J7">
+      <c r="L7">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1990</v>
       </c>
@@ -605,28 +712,36 @@
         <v>230</v>
       </c>
       <c r="C8">
+        <f t="shared" si="0"/>
+        <v>130</v>
+      </c>
+      <c r="D8">
         <v>195</v>
       </c>
-      <c r="D8">
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="F8">
         <v>88</v>
       </c>
-      <c r="E8">
+      <c r="G8">
         <v>63</v>
       </c>
-      <c r="F8">
+      <c r="H8">
         <v>18</v>
       </c>
-      <c r="G8">
+      <c r="I8">
         <v>6</v>
       </c>
-      <c r="H8">
+      <c r="J8">
         <v>450</v>
       </c>
-      <c r="I8">
+      <c r="K8">
         <v>5500</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2005</v>
       </c>
@@ -634,31 +749,39 @@
         <v>240</v>
       </c>
       <c r="C9">
+        <f t="shared" si="0"/>
+        <v>140</v>
+      </c>
+      <c r="D9">
         <v>220</v>
       </c>
-      <c r="D9">
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+      <c r="F9">
         <v>84</v>
       </c>
-      <c r="E9">
+      <c r="G9">
         <v>63</v>
       </c>
-      <c r="F9">
+      <c r="H9">
         <v>17</v>
       </c>
-      <c r="G9">
+      <c r="I9">
         <v>4.5</v>
       </c>
-      <c r="H9">
+      <c r="J9">
         <v>300</v>
       </c>
-      <c r="I9">
+      <c r="K9">
         <v>6000</v>
       </c>
-      <c r="J9">
+      <c r="L9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2014</v>
       </c>
@@ -666,22 +789,30 @@
         <v>250</v>
       </c>
       <c r="C10">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="D10">
         <v>245</v>
       </c>
-      <c r="D10">
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>145</v>
+      </c>
+      <c r="F10">
         <v>83</v>
       </c>
-      <c r="H10">
+      <c r="J10">
         <v>250</v>
       </c>
-      <c r="I10">
+      <c r="K10">
         <v>6500</v>
       </c>
-      <c r="J10">
+      <c r="L10">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2022</v>
       </c>
@@ -689,51 +820,67 @@
         <v>260</v>
       </c>
       <c r="C11">
+        <f t="shared" si="0"/>
+        <v>160</v>
+      </c>
+      <c r="D11">
         <v>260</v>
       </c>
-      <c r="D11">
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="F11">
         <v>82</v>
       </c>
-      <c r="H11">
+      <c r="J11">
         <v>240</v>
       </c>
-      <c r="I11">
+      <c r="K11">
         <v>7500</v>
       </c>
-      <c r="J11">
+      <c r="L11">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" t="s">
         <v>5</v>
       </c>
-      <c r="I13" t="s">
+      <c r="K13" t="s">
         <v>6</v>
       </c>
-      <c r="J13" t="s">
+      <c r="L13" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I17">
+        <f>94/5</f>
+        <v>18.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>